<commit_message>
French Ministories: there seem still to be some problems with the french ministories: I tried to generate and even if there is a ministory with the correct number of forecast i am getting the error Exception in thread "AWT-EventQueue-0" java.lang.NumberFormatException: For input string: "7,76", maybe related to the comma vs period in the number urlTag file: small changes to the URL tag output . New Delimiter: if the text contains commas the text gets separated into several columns... instead of using commas would be good to delimit using something else...change delimiter to slash comma slash ie "\,\" Increase Title Length: could we increase the number of characters you take in the title to 150? (I think now its around 50) MiniStory ID Column: Could you add the ministory id as well as a column? so the column titles would be "miniStoryID,Title,Tag" and the ministoryID column would be empty for non-minstory items
</commit_message>
<xml_diff>
--- a/resources/French/MiniStoryDB/miniStoryDB.xlsx
+++ b/resources/French/MiniStoryDB/miniStoryDB.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielhwang/Documents/OneDrive/Projects/netbeans/NewsLetterAutomation2/resources/French/MiniStoryDB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dariobiasini\Dropbox\Newsletter Automation\NewLetterAutomation(dist)\resources\French\MiniStoryDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$29</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -149,6 +146,15 @@
     </r>
   </si>
   <si>
+    <t>positionType="", mentionsAccuracy="", package1=" " ,package2=" " , package3=" " ,package4=" ", mentionsMarketPremium=""</t>
+  </si>
+  <si>
+    <t>3 jours</t>
+  </si>
+  <si>
+    <t>7 jours</t>
+  </si>
+  <si>
     <r>
       <t>En seulement ###timeFrame###, l'algorithme basé sur l'IA a prédit un retour significatif de ###topReturn11### pour </t>
     </r>
@@ -214,18 +220,30 @@
     <t xml:space="preserve">Les investisseurs ont réalisé un retour significatif en une semaine seulement grâce à ###topStockName11### avec ###topReturn11### de rendement de cette prévision ###packageName1###. De plus, l'algorithme d'I Know First a prédit un retour moyen de près de ###avgReturn21### grâce à cette prévision ###packageName2### avec un niveau d'exactitude équivalent à 90%  En ###timeFrame###, ###topStockName31### a obtenu un retour de ###topReturn21### de ce Package concernant les ###packageName3### qui a connu une prime de marché de plus de ###marketPremium11### sur la même période. </t>
   </si>
   <si>
+    <t>14 jours</t>
+  </si>
+  <si>
     <t xml:space="preserve">En ###timeFrame### les prévisions ont connu des retours exceptionnels pour les investisseurs. ###topStockName11### a augmenté de plus de 80% en accord avec cette ###packageName1###. Les prévisions ont connu un retour moyen de avgReturn11, faisant gagner aux investisseurs environ ###topReturn11### en ###timeFrame###. De plus,###topStockName21### a connu de hauts retours de ###topReturn21### dans cette prévision concernant les ###packageName2###.  Durant ce temps, un investissement passif du S&amp;P 500 rapportait à peine ###snp500Return1### aux investisseurs, démontrant les forts retours obtenus par les prédictions de l'algorithme. </t>
   </si>
   <si>
+    <t>3 mois</t>
+  </si>
+  <si>
     <t>Cette prévision concernant les ###packageName1### a été la plus impressionnante prédiction cette semaine sur timeFrame, avec de hauts retours de ###topStockName11###, ###topStockName12###, et ###topStockName13### avec des retours respectifs de ###topReturn11###, ###topReturn12###, et de ###topReturn13###. Notre prévision concernant les ###packageName2### ont également réalisés de superbes retours avec une moyenne générale de ###avgReturn21###, et des retours significatifs de ###topStockName21### avec près de ###topReturn21###. ###topStockName31### a également gagné un superbe retour de ###topReturn31### en ###timeFrame###, depuis les ###packageName3###. Les prévisions ont eu un niveau d'exactitude de 90% faisant gagner une prime de marché de ###marketPremium31### aux investisseurs.</t>
   </si>
   <si>
+    <t>1 an</t>
+  </si>
+  <si>
     <t xml:space="preserve">L'algorithme autodidacte a prévu des retours sur ###timeFrame### excellents pour ###topStockName11###, ###topStockName12###, ###topStockName13###, and ###topStockName14###, avec des retours respectifs de ###topReturn11###, ###topReturn12###, ###topReturn13###, et ###topReturn14###. Ces hauts retours sont provenus de ###packageName1###. De plus, les prévisions concernant le ###packageName2### ont connu une exactitude de 90% et une moyenne générale de ###avgReturn21### contre un retour S&amp;P 500 de ###snp500Return2###. En ###timeFrame###, ###topStockName21### a connu une croissance de ###topReturn21###, doublant les retours des investisseurs pour cette prévision. Avec un niveau d'exactitude de 100% ces prévisions concernant le ###packageName3###, obtenant des retours de plus de ###topReturn31### avec ###topStockName31###. Ces prévisions ont obtenu une moyenne générale significative de ###avgReturn31### en ###timeFrame###. </t>
   </si>
   <si>
     <t>Les indicateurs algorithmiques d'I Know First peuvent être utilisées pour des stratégies de trading variées. La meilleure stratégie a obtenu un retour de 62.2% alpha au-dessus de l'index S&amp;P500, de Janvier, 2016 jusqu'au 1er Février 2017. Lire le rapport pour plus de détails.</t>
   </si>
   <si>
+    <t>1 mois</t>
+  </si>
+  <si>
     <t xml:space="preserve">Récemment, UPSIDE a mis à l'honneur I Know First dans une explication sur comment prédire les marchés financiers en utilisant le Big Data et l'Intelligence Artificielle. De plus, à l'occasion du Deep Learning In Finance Summit in Singapore de 2017, les co-fondateurs d'I Know First seront conférenciers. Ils vont discuter de la manière dont I Know First utilise les techniques d'apprentissage pour prédire les marchés financiers. </t>
   </si>
   <si>
@@ -1769,35 +1787,14 @@
       </rPr>
       <t/>
     </r>
-  </si>
-  <si>
-    <t>1 an</t>
-  </si>
-  <si>
-    <t>positionType="", mentionsAccuracy="", package1=" " ,package2=" " , package3=" " ,package4=" ", mentionsMarketPremium=""</t>
-  </si>
-  <si>
-    <t>1 mois</t>
-  </si>
-  <si>
-    <t>3 jours</t>
-  </si>
-  <si>
-    <t>14 jours</t>
-  </si>
-  <si>
-    <t>3 mois</t>
-  </si>
-  <si>
-    <t>7 jours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1806,13 +1803,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1848,10 +1853,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1913,7 +1930,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1965,7 +1982,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2167,999 +2184,1278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="1" width="8.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="14.5" collapsed="true"/>
+    <col min="1" max="1" style="1" width="8.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="14.44140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="73.1640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="56.1640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.1640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="12.1640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5" collapsed="true"/>
-    <col min="10" max="11" style="1" width="8.83203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="10.1640625" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="8.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="73.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="56.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="12.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="10.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.6640625" collapsed="true"/>
+    <col min="11" max="11" style="1" width="8.88671875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="10.109375" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="2">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2">
+        <v>14</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2">
+        <v>15</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="2">
+        <v>18</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>19</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>20</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="2">
+        <v>20</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2">
+        <v>21</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="2">
+        <v>22</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="2">
+        <v>23</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="1">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="2">
+        <v>24</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="2">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="L25" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2">
+        <v>25</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K26" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L26" s="2">
         <v>36526</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="27" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="2">
+        <v>26</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1">
+      <c r="J27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="L27" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <v>4</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="2">
+        <v>27</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="L28" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="216" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2">
+        <v>28</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K29" s="2">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L29" s="2">
         <v>36526</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1">
-        <v>4</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1">
-        <v>4</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1">
-        <v>4</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="1">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="1">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1">
-        <v>4</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="1">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1">
-        <v>4</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="1">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="1">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="1">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="1">
-        <v>4</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="1">
-        <v>1</v>
-      </c>
-      <c r="L22" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="1">
-        <v>4</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="1">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="1">
-        <v>4</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="1">
-        <v>1</v>
-      </c>
-      <c r="L24" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1">
-        <v>42758</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="1">
-        <v>4</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="1">
-        <v>1</v>
-      </c>
-      <c r="L25" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1">
-        <v>42764</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>26</v>
-      </c>
-      <c r="C27" s="1">
-        <v>42764</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="1">
-        <v>4</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>27</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42764</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="1">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="225" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1">
-        <v>42764</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="1">
-        <v>4</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H29" s="1">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="1">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1">
-        <v>36526</v>
-      </c>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E30" s="2"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E31" s="2"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E32" s="2"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E33" s="2"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E34" s="2"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E35" s="2"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E36" s="2"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E37" s="2"/>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E38" s="2"/>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E39" s="2"/>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E40" s="2"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E41" s="2"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E42" s="2"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E43" s="2"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E44" s="2"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E45" s="2"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E46" s="2"/>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E47" s="2"/>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E48" s="2"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E49" s="2"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E50" s="2"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E51" s="2"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E52" s="2"/>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E53" s="2"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E54" s="2"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E55" s="2"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L62" s="5"/>
+    </row>
+    <row r="63" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L63" s="5"/>
+    </row>
+    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L65" s="5"/>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L66" s="5"/>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L67" s="5"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L68" s="5"/>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L69" s="5"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L81" s="5"/>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L82" s="5"/>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L83" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L29">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="3 mois"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>
     <hyperlink ref="D15" r:id="rId2"/>
     <hyperlink ref="D23" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>